<commit_message>
Zero value to blanks for Stores and Cluster
</commit_message>
<xml_diff>
--- a/DAILY MONITORING PTP, DEPO & REPO REPORT TEMPLATE.xlsx
+++ b/DAILY MONITORING PTP, DEPO & REPO REPORT TEMPLATE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPM\Documents\UPDATE_FILE\ROB BIKE\DAILY_REMARK_REPORT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPM\Documents\UPDATE_FILE\VSCODE\bpi_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78946795-0362-4549-AC04-8C473E488182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC5262D-D7A7-4B39-8108-A4BBE17E1CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{2A8ADC3F-2E9F-4140-9B94-FC883A5D5D26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2A8ADC3F-2E9F-4140-9B94-FC883A5D5D26}"/>
   </bookViews>
   <sheets>
     <sheet name="MONITORING" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Account Name</t>
   </si>
@@ -173,6 +173,27 @@
   </si>
   <si>
     <t>REDEMPTION VALIDITY EXPIRATION (5-10 days) ReCLASS is every 20th</t>
+  </si>
+  <si>
+    <t>001075800118453</t>
+  </si>
+  <si>
+    <t>YAMBAO, DIVINA MERCIA MILYANNE, VIDA</t>
+  </si>
+  <si>
+    <t>PB - BFL CALAPAN</t>
+  </si>
+  <si>
+    <t>SAN VICENTE CALAPAN CITY</t>
+  </si>
+  <si>
+    <t>001075102830885</t>
+  </si>
+  <si>
+    <t>CUASAY, ALJHUN, ARTILLAGA</t>
+  </si>
+  <si>
+    <t>PB - LEMERY</t>
   </si>
 </sst>
 </file>
@@ -182,8 +203,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -292,7 +313,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -304,10 +325,10 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -335,7 +356,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -343,6 +364,17 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -661,9 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB94F83-117B-432F-8D63-CC3C03370F1A}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -740,9 +770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5A34E97-E124-4F7A-9CAA-DAAA7207D842}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -793,24 +821,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{973BA036-E4CF-4A2A-9627-6C5C009CDB08}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -847,6 +873,39 @@
       </c>
       <c r="K1" s="15" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="20">
+        <v>9258.61</v>
+      </c>
+      <c r="E2" s="21">
+        <v>45744</v>
+      </c>
+      <c r="F2" s="9">
+        <v>262</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="22">
+        <v>45779</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -856,11 +915,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE18C21A-B9E0-43B9-B7FF-D995E8EB6C28}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -904,6 +961,35 @@
         <v>45</v>
       </c>
     </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="23">
+        <v>51435.57</v>
+      </c>
+      <c r="E2" s="22">
+        <v>45754</v>
+      </c>
+      <c r="F2" s="9">
+        <v>238</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="22">
+        <v>45773</v>
+      </c>
+      <c r="I2" s="22">
+        <v>45783</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -913,9 +999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B65FBB-96EC-47F7-A70D-A89DA7E85025}">
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>